<commit_message>
Init on emissions data handling
</commit_message>
<xml_diff>
--- a/Datamall.xlsx
+++ b/Datamall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.gustafsson\Jupyter Notebooks\GHG Reporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.gustafsson\Jupyter Notebooks\ghg-reporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84925378-3EC5-4B59-BB3F-C788856C8B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFBB9D7-1A73-460D-B6DF-940673DC9209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{20C734F0-5E67-4AA5-9DDA-63BA682F1DC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{20C734F0-5E67-4AA5-9DDA-63BA682F1DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Aktivitet</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Aktivitetsdata</t>
+  </si>
+  <si>
+    <t>Atkvitetsdata</t>
+  </si>
+  <si>
+    <t>Emissionsfaktor</t>
   </si>
 </sst>
 </file>
@@ -206,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -352,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -528,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580CA44D-2B43-489A-B99D-BC7434C19246}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,24 +614,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9C05BB0-1E80-4825-985E-3A71AA908701}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>